<commit_message>
Beginning of ATO Datawarehouse design, fact sheet
Added additional columns for the beginning of datawarehouse. Notice column titled 'Item Code'. A seperate excel sheet of the names of all items, and a code number (start from 1 and go forward) should be created.
</commit_message>
<xml_diff>
--- a/Material Purhcase for Dr. Berglund Paint job.xlsx
+++ b/Material Purhcase for Dr. Berglund Paint job.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niketa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymo\Dropbox\GitHub\ATO-Contracting-LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF07267-9F4D-4220-8353-80E4FA3782AF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CDB592-AC87-429A-9A07-0351AF94D691}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{817413F5-5CE5-4C8F-808D-E67FB2CE72C2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="391">
   <si>
     <t>1/4" T50 STAPLES 5000 CT 504IP</t>
   </si>
@@ -1131,15 +1131,9 @@
     <t xml:space="preserve">2434108 4@$3.98 </t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
-    <t>qty</t>
-  </si>
-  <si>
     <t>10" BS COMF TAPING KNIFE 3661</t>
   </si>
   <si>
@@ -1189,6 +1183,27 @@
   </si>
   <si>
     <t>Column4</t>
+  </si>
+  <si>
+    <t>Return (0=no, 1= yes)</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Item Code: 1=Tool, 2=Job Material, 3=Job NonDurable</t>
+  </si>
+  <si>
+    <t>End of Job Accounted, 0 = no, 1= yes</t>
+  </si>
+  <si>
+    <t>Work Type (paint, drywall)</t>
+  </si>
+  <si>
+    <t>Item  Code</t>
   </si>
 </sst>
 </file>
@@ -3611,48 +3626,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2264771-1839-4E11-8C15-34168CA9BAF2}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:I199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E200" sqref="E200"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="68.85546875" customWidth="1"/>
+    <col min="8" max="8" width="48.140625" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3666,8 +3702,9 @@
         <f>A3*C3</f>
         <v>9.98</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3681,13 +3718,14 @@
         <f t="shared" ref="D4:D67" si="0">A4*C4</f>
         <v>2.4900000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C5" s="7">
         <v>7.98</v>
@@ -3696,8 +3734,9 @@
         <f t="shared" si="0"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3711,8 +3750,9 @@
         <f t="shared" si="0"/>
         <v>15.92</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3726,8 +3766,9 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3741,8 +3782,9 @@
         <f t="shared" si="0"/>
         <v>6.58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3756,8 +3798,9 @@
         <f t="shared" si="0"/>
         <v>19.88</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3771,8 +3814,9 @@
         <f t="shared" si="0"/>
         <v>19.88</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3786,8 +3830,9 @@
         <f t="shared" si="0"/>
         <v>3.98</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -3801,8 +3846,9 @@
         <f t="shared" si="0"/>
         <v>49.99</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3816,8 +3862,9 @@
         <f t="shared" si="0"/>
         <v>16.62</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3831,8 +3878,9 @@
         <f t="shared" si="0"/>
         <v>3.59</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -3846,8 +3894,9 @@
         <f t="shared" si="0"/>
         <v>3.59</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3861,8 +3910,9 @@
         <f t="shared" si="0"/>
         <v>7.18</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3876,8 +3926,9 @@
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3891,8 +3942,9 @@
         <f t="shared" si="0"/>
         <v>9.99</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -3906,8 +3958,9 @@
         <f t="shared" si="0"/>
         <v>10.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -3921,8 +3974,9 @@
         <f t="shared" si="0"/>
         <v>20.94</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -3936,8 +3990,9 @@
         <f t="shared" si="0"/>
         <v>5.68</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3951,8 +4006,9 @@
         <f t="shared" si="0"/>
         <v>5.91</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3966,8 +4022,9 @@
         <f t="shared" si="0"/>
         <v>7.99</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3981,8 +4038,9 @@
         <f t="shared" si="0"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3996,8 +4054,9 @@
         <f t="shared" si="0"/>
         <v>38.97</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4011,8 +4070,9 @@
         <f t="shared" si="0"/>
         <v>5.98</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -4026,8 +4086,9 @@
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -4041,8 +4102,9 @@
         <f t="shared" si="0"/>
         <v>9.99</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4056,13 +4118,14 @@
         <f t="shared" si="0"/>
         <v>4.29</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C30" s="7">
         <v>13.48</v>
@@ -4071,13 +4134,14 @@
         <f t="shared" si="0"/>
         <v>67.400000000000006</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C31" s="7">
         <v>8.91</v>
@@ -4086,13 +4150,14 @@
         <f t="shared" si="0"/>
         <v>17.82</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C32" s="7">
         <v>11.97</v>
@@ -4101,13 +4166,14 @@
         <f t="shared" si="0"/>
         <v>11.97</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C33" s="7">
         <v>3.49</v>
@@ -4116,13 +4182,14 @@
         <f t="shared" si="0"/>
         <v>3.49</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C34" s="7">
         <v>9.99</v>
@@ -4131,8 +4198,9 @@
         <f t="shared" si="0"/>
         <v>19.98</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4146,8 +4214,9 @@
         <f t="shared" si="0"/>
         <v>3.38</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -4161,8 +4230,9 @@
         <f t="shared" si="0"/>
         <v>59.94</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -4176,8 +4246,9 @@
         <f t="shared" si="0"/>
         <v>8.9700000000000006</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -4191,13 +4262,14 @@
         <f t="shared" si="0"/>
         <v>6.99</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C39" s="7">
         <v>7.89</v>
@@ -4206,13 +4278,14 @@
         <f t="shared" si="0"/>
         <v>31.56</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C40" s="7">
         <v>7.99</v>
@@ -4221,13 +4294,14 @@
         <f t="shared" si="0"/>
         <v>15.98</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C41" s="7">
         <v>8.98</v>
@@ -4236,8 +4310,9 @@
         <f t="shared" si="0"/>
         <v>8.98</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -4251,8 +4326,9 @@
         <f t="shared" si="0"/>
         <v>9.99</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5</v>
       </c>
@@ -4266,8 +4342,9 @@
         <f t="shared" si="0"/>
         <v>67.400000000000006</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -4281,8 +4358,9 @@
         <f t="shared" si="0"/>
         <v>59.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -4296,8 +4374,9 @@
         <f t="shared" si="0"/>
         <v>9.9600000000000009</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -4311,8 +4390,9 @@
         <f t="shared" si="0"/>
         <v>29.28</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -4326,8 +4406,9 @@
         <f t="shared" si="0"/>
         <v>33.97</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -4341,8 +4422,9 @@
         <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -4356,8 +4438,9 @@
         <f t="shared" si="0"/>
         <v>19.760000000000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -4371,8 +4454,9 @@
         <f t="shared" si="0"/>
         <v>2.89</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -4386,8 +4470,9 @@
         <f t="shared" si="0"/>
         <v>9.99</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -4401,8 +4486,9 @@
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="7"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -4416,8 +4502,9 @@
         <f t="shared" si="0"/>
         <v>65.94</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="7"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -4431,8 +4518,9 @@
         <f t="shared" si="0"/>
         <v>5.59</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="7"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -4446,8 +4534,9 @@
         <f t="shared" si="0"/>
         <v>8.7799999999999994</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -4461,8 +4550,9 @@
         <f t="shared" si="0"/>
         <v>4.8899999999999997</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -4476,8 +4566,9 @@
         <f t="shared" si="0"/>
         <v>9.98</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -4491,8 +4582,9 @@
         <f t="shared" si="0"/>
         <v>21.96</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -4506,8 +4598,9 @@
         <f t="shared" si="0"/>
         <v>19.97</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -4521,8 +4614,9 @@
         <f t="shared" si="0"/>
         <v>2.39</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1</v>
       </c>
@@ -4536,8 +4630,9 @@
         <f t="shared" si="0"/>
         <v>7.99</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -4551,8 +4646,9 @@
         <f t="shared" si="0"/>
         <v>29.98</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5</v>
       </c>
@@ -4566,8 +4662,9 @@
         <f t="shared" si="0"/>
         <v>12.450000000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4581,8 +4678,9 @@
         <f t="shared" si="0"/>
         <v>4.58</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1</v>
       </c>
@@ -4596,8 +4694,9 @@
         <f t="shared" si="0"/>
         <v>59.99</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4611,8 +4710,9 @@
         <f t="shared" si="0"/>
         <v>15.96</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1</v>
       </c>
@@ -4626,8 +4726,9 @@
         <f t="shared" si="0"/>
         <v>3.69</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -4641,8 +4742,9 @@
         <f t="shared" ref="D68:D199" si="1">A68*C68</f>
         <v>3.99</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="7"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
       </c>
@@ -4656,8 +4758,9 @@
         <f t="shared" si="1"/>
         <v>1.89</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="7"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1</v>
       </c>
@@ -4671,8 +4774,9 @@
         <f t="shared" si="1"/>
         <v>1.89</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="7"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1</v>
       </c>
@@ -4686,8 +4790,9 @@
         <f t="shared" si="1"/>
         <v>1.69</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1</v>
       </c>
@@ -4701,8 +4806,9 @@
         <f t="shared" si="1"/>
         <v>3.69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="7"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1</v>
       </c>
@@ -4716,8 +4822,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="7"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1</v>
       </c>
@@ -4731,13 +4838,14 @@
         <f t="shared" si="1"/>
         <v>29.95</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E74" s="7"/>
+    </row>
+    <row r="75" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C75" s="7">
         <v>3.84</v>
@@ -4746,13 +4854,14 @@
         <f t="shared" si="1"/>
         <v>11.52</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="7"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>10</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C76" s="11">
         <v>4.8899999999999997</v>
@@ -4761,8 +4870,9 @@
         <f t="shared" si="1"/>
         <v>48.9</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="12"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1</v>
       </c>
@@ -4776,8 +4886,9 @@
         <f t="shared" si="1"/>
         <v>8.7799999999999994</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1</v>
       </c>
@@ -4791,8 +4902,9 @@
         <f t="shared" si="1"/>
         <v>4.99</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -4806,8 +4918,9 @@
         <f t="shared" si="1"/>
         <v>8.94</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1</v>
       </c>
@@ -4821,8 +4934,9 @@
         <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="7"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1</v>
       </c>
@@ -4836,8 +4950,9 @@
         <f t="shared" si="1"/>
         <v>2.09</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1</v>
       </c>
@@ -4851,8 +4966,9 @@
         <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1</v>
       </c>
@@ -4866,8 +4982,9 @@
         <f t="shared" si="1"/>
         <v>0.99</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1</v>
       </c>
@@ -4881,8 +4998,9 @@
         <f t="shared" si="1"/>
         <v>2.94</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="7"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1</v>
       </c>
@@ -4896,8 +5014,9 @@
         <f t="shared" si="1"/>
         <v>0.87</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="7"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1</v>
       </c>
@@ -4911,8 +5030,9 @@
         <f t="shared" si="1"/>
         <v>0.49</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1</v>
       </c>
@@ -4926,8 +5046,9 @@
         <f t="shared" si="1"/>
         <v>0.49</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2</v>
       </c>
@@ -4941,8 +5062,9 @@
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="7"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1</v>
       </c>
@@ -4956,8 +5078,9 @@
         <f t="shared" si="1"/>
         <v>13.88</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="7"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1</v>
       </c>
@@ -4971,8 +5094,9 @@
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="7"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1</v>
       </c>
@@ -4986,8 +5110,9 @@
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="7"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -5001,8 +5126,9 @@
         <f t="shared" si="1"/>
         <v>1.29</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="7"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -5016,8 +5142,9 @@
         <f t="shared" si="1"/>
         <v>13.88</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="7"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1</v>
       </c>
@@ -5031,8 +5158,9 @@
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="7"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2</v>
       </c>
@@ -5046,8 +5174,9 @@
         <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="7"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4</v>
       </c>
@@ -5061,8 +5190,9 @@
         <f t="shared" si="1"/>
         <v>15.36</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="7"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2</v>
       </c>
@@ -5076,8 +5206,9 @@
         <f t="shared" si="1"/>
         <v>9.74</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="7"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1</v>
       </c>
@@ -5091,8 +5222,9 @@
         <f t="shared" si="1"/>
         <v>21.98</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="7"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -5106,8 +5238,9 @@
         <f t="shared" si="1"/>
         <v>14.98</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="7"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1</v>
       </c>
@@ -5121,8 +5254,9 @@
         <f t="shared" si="1"/>
         <v>4.4800000000000004</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="7"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4</v>
       </c>
@@ -5136,8 +5270,9 @@
         <f t="shared" si="1"/>
         <v>7.96</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="7"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2</v>
       </c>
@@ -5151,8 +5286,9 @@
         <f t="shared" si="1"/>
         <v>5.94</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="7"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1</v>
       </c>
@@ -5166,8 +5302,9 @@
         <f t="shared" si="1"/>
         <v>6.97</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="7"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1</v>
       </c>
@@ -5181,8 +5318,9 @@
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>4</v>
       </c>
@@ -5196,8 +5334,9 @@
         <f t="shared" si="1"/>
         <v>15.96</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="7"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2</v>
       </c>
@@ -5211,8 +5350,9 @@
         <f t="shared" si="1"/>
         <v>5.98</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1</v>
       </c>
@@ -5226,8 +5366,9 @@
         <f t="shared" si="1"/>
         <v>39.979999999999997</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2</v>
       </c>
@@ -5241,8 +5382,9 @@
         <f t="shared" si="1"/>
         <v>2.94</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2</v>
       </c>
@@ -5256,8 +5398,9 @@
         <f t="shared" si="1"/>
         <v>9.7799999999999994</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2</v>
       </c>
@@ -5271,8 +5414,9 @@
         <f t="shared" si="1"/>
         <v>19.98</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2</v>
       </c>
@@ -5286,8 +5430,9 @@
         <f t="shared" si="1"/>
         <v>27.98</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="7"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1</v>
       </c>
@@ -5301,8 +5446,9 @@
         <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="7"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1</v>
       </c>
@@ -5316,8 +5462,9 @@
         <f t="shared" si="1"/>
         <v>9.94</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="7"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>4</v>
       </c>
@@ -5331,8 +5478,9 @@
         <f t="shared" si="1"/>
         <v>7.16</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="7"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2</v>
       </c>
@@ -5346,8 +5494,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="7"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1</v>
       </c>
@@ -5361,8 +5510,9 @@
         <f t="shared" si="1"/>
         <v>14.85</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="7"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2</v>
       </c>
@@ -5376,8 +5526,9 @@
         <f t="shared" si="1"/>
         <v>5.94</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1</v>
       </c>
@@ -5391,8 +5542,9 @@
         <f t="shared" si="1"/>
         <v>21.98</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="7"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>3</v>
       </c>
@@ -5406,8 +5558,9 @@
         <f t="shared" si="1"/>
         <v>11.97</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="7"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1</v>
       </c>
@@ -5421,8 +5574,9 @@
         <f t="shared" si="1"/>
         <v>2.4900000000000002</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1</v>
       </c>
@@ -5436,8 +5590,9 @@
         <f t="shared" si="1"/>
         <v>6.99</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="7"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1</v>
       </c>
@@ -5451,8 +5606,9 @@
         <f t="shared" si="1"/>
         <v>4.99</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="7"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1</v>
       </c>
@@ -5466,8 +5622,9 @@
         <f t="shared" si="1"/>
         <v>14.97</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="7"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1</v>
       </c>
@@ -5481,8 +5638,9 @@
         <f t="shared" si="1"/>
         <v>7.49</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="7"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1</v>
       </c>
@@ -5496,8 +5654,9 @@
         <f t="shared" si="1"/>
         <v>1.89</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="7"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>3</v>
       </c>
@@ -5511,8 +5670,9 @@
         <f t="shared" si="1"/>
         <v>8.370000000000001</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="7"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2</v>
       </c>
@@ -5526,8 +5686,9 @@
         <f t="shared" si="1"/>
         <v>8.34</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="7"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2</v>
       </c>
@@ -5541,8 +5702,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1</v>
       </c>
@@ -5556,8 +5718,9 @@
         <f t="shared" si="1"/>
         <v>2.97</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="7"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1</v>
       </c>
@@ -5571,8 +5734,9 @@
         <f t="shared" si="1"/>
         <v>6.97</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="7"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2</v>
       </c>
@@ -5586,8 +5750,9 @@
         <f t="shared" si="1"/>
         <v>13.52</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1</v>
       </c>
@@ -5601,8 +5766,9 @@
         <f t="shared" si="1"/>
         <v>35.979999999999997</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2</v>
       </c>
@@ -5616,8 +5782,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="7"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1</v>
       </c>
@@ -5631,8 +5798,9 @@
         <f t="shared" si="1"/>
         <v>35.979999999999997</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="7"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2</v>
       </c>
@@ -5646,8 +5814,9 @@
         <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1</v>
       </c>
@@ -5661,8 +5830,9 @@
         <f t="shared" si="1"/>
         <v>12.49</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1</v>
       </c>
@@ -5676,8 +5846,9 @@
         <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2</v>
       </c>
@@ -5691,8 +5862,9 @@
         <f t="shared" si="1"/>
         <v>13.96</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2</v>
       </c>
@@ -5706,8 +5878,9 @@
         <f t="shared" si="1"/>
         <v>13.96</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1</v>
       </c>
@@ -5721,8 +5894,9 @@
         <f t="shared" si="1"/>
         <v>29.95</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2</v>
       </c>
@@ -5736,8 +5910,9 @@
         <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2</v>
       </c>
@@ -5751,8 +5926,9 @@
         <f t="shared" si="1"/>
         <v>3.96</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1</v>
       </c>
@@ -5766,8 +5942,9 @@
         <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1</v>
       </c>
@@ -5781,8 +5958,9 @@
         <f t="shared" si="1"/>
         <v>5.97</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1</v>
       </c>
@@ -5796,8 +5974,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1</v>
       </c>
@@ -5811,8 +5990,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1</v>
       </c>
@@ -5826,8 +6006,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="7"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1</v>
       </c>
@@ -5841,8 +6022,9 @@
         <f t="shared" si="1"/>
         <v>1.99</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="7"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2</v>
       </c>
@@ -5856,8 +6038,9 @@
         <f t="shared" si="1"/>
         <v>7.56</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1</v>
       </c>
@@ -5871,8 +6054,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1</v>
       </c>
@@ -5886,8 +6070,9 @@
         <f t="shared" si="1"/>
         <v>3.78</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1</v>
       </c>
@@ -5901,8 +6086,9 @@
         <f t="shared" si="1"/>
         <v>28.64</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1</v>
       </c>
@@ -5916,8 +6102,9 @@
         <f t="shared" si="1"/>
         <v>28.64</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1</v>
       </c>
@@ -5931,8 +6118,9 @@
         <f t="shared" si="1"/>
         <v>3.88</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="7"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1</v>
       </c>
@@ -5946,8 +6134,9 @@
         <f t="shared" si="1"/>
         <v>2.46</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1</v>
       </c>
@@ -5961,8 +6150,9 @@
         <f t="shared" si="1"/>
         <v>2.97</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="7"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2</v>
       </c>
@@ -5976,8 +6166,9 @@
         <f t="shared" si="1"/>
         <v>7.98</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="7"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1</v>
       </c>
@@ -5991,8 +6182,9 @@
         <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1</v>
       </c>
@@ -6006,8 +6198,9 @@
         <f t="shared" si="1"/>
         <v>4.97</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1</v>
       </c>
@@ -6021,8 +6214,9 @@
         <f t="shared" si="1"/>
         <v>7.96</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>4</v>
       </c>
@@ -6036,8 +6230,9 @@
         <f t="shared" si="1"/>
         <v>7.96</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="7"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1</v>
       </c>
@@ -6051,8 +6246,9 @@
         <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="7"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1</v>
       </c>
@@ -6066,8 +6262,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="7"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1</v>
       </c>
@@ -6081,8 +6278,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1</v>
       </c>
@@ -6096,8 +6294,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1</v>
       </c>
@@ -6111,8 +6310,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1</v>
       </c>
@@ -6126,8 +6326,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1</v>
       </c>
@@ -6141,8 +6342,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1</v>
       </c>
@@ -6156,8 +6358,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169" s="7"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1</v>
       </c>
@@ -6171,13 +6374,14 @@
         <f t="shared" si="1"/>
         <v>7.96</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170" s="7"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1</v>
       </c>
       <c r="B171" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C171" s="7">
         <v>4.9800000000000004</v>
@@ -6186,8 +6390,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171" s="7"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1</v>
       </c>
@@ -6201,8 +6406,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172" s="7"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1</v>
       </c>
@@ -6216,8 +6422,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" s="7"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1</v>
       </c>
@@ -6231,8 +6438,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174" s="7"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1</v>
       </c>
@@ -6246,8 +6454,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175" s="7"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1</v>
       </c>
@@ -6261,8 +6470,9 @@
         <f t="shared" si="1"/>
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" s="7"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1</v>
       </c>
@@ -6276,8 +6486,9 @@
         <f t="shared" si="1"/>
         <v>15.97</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" s="7"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1</v>
       </c>
@@ -6291,8 +6502,9 @@
         <f t="shared" si="1"/>
         <v>7.29</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" s="7"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1</v>
       </c>
@@ -6306,8 +6518,9 @@
         <f t="shared" si="1"/>
         <v>28.64</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="7"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1</v>
       </c>
@@ -6321,8 +6534,9 @@
         <f t="shared" si="1"/>
         <v>3.29</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" s="7"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1</v>
       </c>
@@ -6336,8 +6550,9 @@
         <f t="shared" si="1"/>
         <v>8.99</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181" s="7"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1</v>
       </c>
@@ -6351,8 +6566,9 @@
         <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182" s="7"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1</v>
       </c>
@@ -6366,8 +6582,9 @@
         <f t="shared" si="1"/>
         <v>2.98</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183" s="7"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1</v>
       </c>
@@ -6381,8 +6598,9 @@
         <f t="shared" si="1"/>
         <v>29.99</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="7"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1</v>
       </c>
@@ -6396,8 +6614,9 @@
         <f t="shared" si="1"/>
         <v>4.99</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" s="7"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>2</v>
       </c>
@@ -6411,8 +6630,9 @@
         <f t="shared" si="1"/>
         <v>3.96</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" s="7"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2</v>
       </c>
@@ -6426,8 +6646,9 @@
         <f t="shared" si="1"/>
         <v>3.38</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="7"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1</v>
       </c>
@@ -6441,8 +6662,9 @@
         <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" s="7"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>2</v>
       </c>
@@ -6456,8 +6678,9 @@
         <f t="shared" si="1"/>
         <v>1.64</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189" s="7"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1</v>
       </c>
@@ -6471,8 +6694,9 @@
         <f t="shared" si="1"/>
         <v>0.82</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" s="7"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1</v>
       </c>
@@ -6486,8 +6710,9 @@
         <f t="shared" si="1"/>
         <v>29.99</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" s="7"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1</v>
       </c>
@@ -6501,8 +6726,9 @@
         <f t="shared" si="1"/>
         <v>2.89</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="7"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1</v>
       </c>
@@ -6516,8 +6742,9 @@
         <f t="shared" si="1"/>
         <v>2.97</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193" s="7"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>1</v>
       </c>
@@ -6531,8 +6758,9 @@
         <f t="shared" si="1"/>
         <v>5.85</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194" s="7"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1</v>
       </c>
@@ -6546,8 +6774,9 @@
         <f t="shared" si="1"/>
         <v>3.98</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195" s="7"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1</v>
       </c>
@@ -6561,8 +6790,9 @@
         <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196" s="7"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>5</v>
       </c>
@@ -6576,8 +6806,9 @@
         <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197" s="7"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>2</v>
       </c>
@@ -6591,8 +6822,9 @@
         <f t="shared" si="1"/>
         <v>1.64</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198" s="7"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2</v>
       </c>
@@ -6606,6 +6838,7 @@
         <f t="shared" si="1"/>
         <v>6.58</v>
       </c>
+      <c r="E199" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>